<commit_message>
Actualizar datos del informe con Excel de DD/MM/AAAA
</commit_message>
<xml_diff>
--- a/02. INFORME CONSUMOS MENSUALES VISIONAMOS.xlsx
+++ b/02. INFORME CONSUMOS MENSUALES VISIONAMOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e406a71730fc9f56/Documentos/INFORME VISIONAMOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{FC691D29-6544-4CAF-A4FF-C1FDB2106A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11FF06F8-A4ED-476D-B490-0B727DB15F21}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{656227FB-19D5-4C5E-AAC2-E1F815816321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{69732437-4200-402F-958C-600D01F3DE1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="33">
   <si>
     <t>ENTIDAD</t>
   </si>
@@ -130,6 +130,12 @@
   <si>
     <t>ANÁLISIS CODEUDOR</t>
   </si>
+  <si>
+    <t>SUPRESENCIA</t>
+  </si>
+  <si>
+    <t>MUTUAL SAN JERONIMO</t>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -555,11 +561,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -664,6 +696,17 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,8 +1294,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AED9E32-47C1-4DC5-9134-96A9E135D850}" name="Tabla1" displayName="Tabla1" ref="A1:G668" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
-  <autoFilter ref="A1:G668" xr:uid="{1AED9E32-47C1-4DC5-9134-96A9E135D850}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AED9E32-47C1-4DC5-9134-96A9E135D850}" name="Tabla1" displayName="Tabla1" ref="A1:G689" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+  <autoFilter ref="A1:G689" xr:uid="{1AED9E32-47C1-4DC5-9134-96A9E135D850}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{C1FF5726-9C48-4578-8EB2-662910221D0B}" name="MES" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="2" xr3:uid="{CD9D771F-FF5C-4793-AD6F-514DCA7408F3}" name="AÑO" dataDxfId="11" totalsRowDxfId="10"/>
@@ -1585,11 +1628,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4067E17-64EB-4E86-B6C6-C322909CE277}">
-  <dimension ref="A1:I668"/>
+  <dimension ref="A1:I689"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A510" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G544" sqref="G544:G560"/>
+      <pane ySplit="1" topLeftCell="A675" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I686" sqref="I686"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17610,7 +17653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A668" s="55">
         <v>45962</v>
       </c>
@@ -17632,6 +17675,506 @@
       <c r="G668" s="43">
         <f t="shared" si="87"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A669" s="56">
+        <v>45992</v>
+      </c>
+      <c r="B669" s="8">
+        <v>2025</v>
+      </c>
+      <c r="C669" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D669" s="57">
+        <v>0</v>
+      </c>
+      <c r="E669" s="57">
+        <v>6</v>
+      </c>
+      <c r="F669" s="57">
+        <v>0</v>
+      </c>
+      <c r="G669" s="58">
+        <f>E669+F669</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A670" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B670" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C670" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D670" s="13">
+        <v>0</v>
+      </c>
+      <c r="E670" s="13">
+        <v>154</v>
+      </c>
+      <c r="F670" s="13">
+        <v>18</v>
+      </c>
+      <c r="G670" s="60">
+        <f t="shared" ref="G670:G672" si="89">E670+F670</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A671" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B671" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C671" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D671" s="13">
+        <v>0</v>
+      </c>
+      <c r="E671" s="13">
+        <v>52</v>
+      </c>
+      <c r="F671" s="13">
+        <v>16</v>
+      </c>
+      <c r="G671" s="60">
+        <f t="shared" si="89"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A672" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B672" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C672" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D672" s="13">
+        <v>0</v>
+      </c>
+      <c r="E672" s="13">
+        <v>30</v>
+      </c>
+      <c r="F672" s="13">
+        <v>4</v>
+      </c>
+      <c r="G672" s="60">
+        <f t="shared" si="89"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A673" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B673" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C673" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D673" s="13">
+        <v>0</v>
+      </c>
+      <c r="E673" s="13">
+        <v>0</v>
+      </c>
+      <c r="F673" s="13">
+        <v>0</v>
+      </c>
+      <c r="G673" s="60">
+        <f>E673+F673</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A674" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B674" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C674" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D674" s="13">
+        <v>0</v>
+      </c>
+      <c r="E674" s="13">
+        <v>8</v>
+      </c>
+      <c r="F674" s="13">
+        <v>3</v>
+      </c>
+      <c r="G674" s="60">
+        <f>E674+F674</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="675" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A675" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B675" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C675" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D675" s="13">
+        <v>0</v>
+      </c>
+      <c r="E675" s="13">
+        <v>1</v>
+      </c>
+      <c r="F675" s="13">
+        <v>1</v>
+      </c>
+      <c r="G675" s="60">
+        <f t="shared" ref="G675:G679" si="90">E675+F675</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="676" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A676" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B676" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C676" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D676" s="13">
+        <v>0</v>
+      </c>
+      <c r="E676" s="13"/>
+      <c r="F676" s="13"/>
+      <c r="G676" s="60">
+        <f t="shared" si="90"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A677" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B677" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C677" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D677" s="13">
+        <v>1</v>
+      </c>
+      <c r="E677" s="13">
+        <v>1</v>
+      </c>
+      <c r="F677" s="13">
+        <v>0</v>
+      </c>
+      <c r="G677" s="60">
+        <f t="shared" si="90"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A678" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B678" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C678" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D678" s="13">
+        <v>0</v>
+      </c>
+      <c r="E678" s="13">
+        <v>12</v>
+      </c>
+      <c r="F678" s="13">
+        <v>2</v>
+      </c>
+      <c r="G678" s="60">
+        <f t="shared" si="90"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="679" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A679" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B679" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C679" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D679" s="13">
+        <v>0</v>
+      </c>
+      <c r="E679" s="13">
+        <v>101</v>
+      </c>
+      <c r="F679" s="13">
+        <v>1</v>
+      </c>
+      <c r="G679" s="60">
+        <f t="shared" si="90"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="680" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A680" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B680" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C680" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D680" s="13">
+        <v>1</v>
+      </c>
+      <c r="E680" s="13">
+        <v>6</v>
+      </c>
+      <c r="F680" s="13">
+        <v>0</v>
+      </c>
+      <c r="G680" s="60">
+        <f>E680+F680</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="681" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A681" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B681" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C681" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D681" s="13">
+        <v>0</v>
+      </c>
+      <c r="E681" s="13">
+        <v>5</v>
+      </c>
+      <c r="F681" s="13">
+        <v>0</v>
+      </c>
+      <c r="G681" s="60">
+        <f>E681+F681</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="682" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A682" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B682" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C682" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D682" s="13">
+        <v>0</v>
+      </c>
+      <c r="E682" s="13">
+        <v>6</v>
+      </c>
+      <c r="F682" s="13">
+        <v>0</v>
+      </c>
+      <c r="G682" s="60">
+        <f>E682+F682</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="683" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A683" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B683" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C683" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D683" s="13">
+        <v>1</v>
+      </c>
+      <c r="E683" s="13">
+        <v>11</v>
+      </c>
+      <c r="F683" s="13">
+        <v>0</v>
+      </c>
+      <c r="G683" s="60">
+        <f t="shared" ref="G683:G688" si="91">E683+F683</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A684" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B684" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C684" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D684" s="13">
+        <v>0</v>
+      </c>
+      <c r="E684" s="13">
+        <v>27</v>
+      </c>
+      <c r="F684" s="13">
+        <v>0</v>
+      </c>
+      <c r="G684" s="60">
+        <f t="shared" si="91"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="685" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A685" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B685" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C685" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D685" s="13">
+        <v>0</v>
+      </c>
+      <c r="E685" s="13">
+        <v>0</v>
+      </c>
+      <c r="F685" s="13">
+        <v>0</v>
+      </c>
+      <c r="G685" s="60">
+        <f>E685+F685</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="686" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A686" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B686" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C686" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D686" s="13">
+        <v>0</v>
+      </c>
+      <c r="E686" s="13">
+        <v>0</v>
+      </c>
+      <c r="F686" s="13">
+        <v>0</v>
+      </c>
+      <c r="G686" s="60">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A687" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B687" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C687" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D687" s="13">
+        <v>0</v>
+      </c>
+      <c r="E687" s="13">
+        <v>0</v>
+      </c>
+      <c r="F687" s="13">
+        <v>0</v>
+      </c>
+      <c r="G687" s="60">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A688" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B688" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C688" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D688" s="13">
+        <v>0</v>
+      </c>
+      <c r="E688" s="13">
+        <v>7</v>
+      </c>
+      <c r="F688" s="13">
+        <v>0</v>
+      </c>
+      <c r="G688" s="60">
+        <f t="shared" si="91"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A689" s="59">
+        <v>45992</v>
+      </c>
+      <c r="B689" s="12">
+        <v>2025</v>
+      </c>
+      <c r="C689" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D689" s="13">
+        <v>0</v>
+      </c>
+      <c r="E689" s="13">
+        <v>4</v>
+      </c>
+      <c r="F689" s="13">
+        <v>0</v>
+      </c>
+      <c r="G689" s="60">
+        <f>E689+F689</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>